<commit_message>
Terminata valutazione e documentazione
</commit_message>
<xml_diff>
--- a/doc/valutazione.xlsx
+++ b/doc/valutazione.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodolfo Pio Sassone\eclipse-workspace\Tressette\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F315DE47-F2C9-406E-81AB-E9EA8DD239F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF87B788-4B78-4C91-8986-B6C13EC9F31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{88201FB0-324F-4AAE-9D56-D0CDBF2B8877}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{88201FB0-324F-4AAE-9D56-D0CDBF2B8877}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulazioni" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="17">
   <si>
     <t>avv1</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>Mazzo</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>M7</t>
+  </si>
+  <si>
+    <t>M8</t>
   </si>
 </sst>
 </file>
@@ -313,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -359,16 +371,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -377,15 +398,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,64 +713,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB1E0673-BD1D-4988-8A91-BAB1C750EC06}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AQ24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="16">
         <v>1</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
-      <c r="F1" s="24"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="15">
         <v>2</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
-      <c r="J1" s="24"/>
+      <c r="J1" s="17"/>
       <c r="K1" s="15">
         <v>3</v>
       </c>
       <c r="L1" s="16"/>
       <c r="M1" s="16"/>
-      <c r="N1" s="24"/>
+      <c r="N1" s="17"/>
       <c r="O1" s="15">
         <v>4</v>
       </c>
       <c r="P1" s="16"/>
       <c r="Q1" s="16"/>
-      <c r="R1" s="24"/>
+      <c r="R1" s="17"/>
       <c r="S1" s="15">
         <v>5</v>
       </c>
       <c r="T1" s="16"/>
       <c r="U1" s="16"/>
-      <c r="V1" s="24"/>
+      <c r="V1" s="17"/>
       <c r="W1" s="15">
         <v>6</v>
       </c>
       <c r="X1" s="16"/>
       <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="15">
+        <v>7</v>
+      </c>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="15">
+        <v>8</v>
+      </c>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="15">
+        <v>9</v>
+      </c>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="15">
+        <v>10</v>
+      </c>
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="16"/>
+      <c r="AP1" s="17"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
@@ -827,11 +867,59 @@
       <c r="Y2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="AA2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -905,157 +993,354 @@
       <c r="Y3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="Z3" s="13" t="s">
         <v>7</v>
       </c>
+      <c r="AA3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:43" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="19">
         <v>10</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19">
         <v>1</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="17">
+      <c r="F4" s="20"/>
+      <c r="G4" s="18">
         <v>7</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18">
+      <c r="H4" s="19"/>
+      <c r="I4" s="19">
         <v>4</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="17">
+      <c r="J4" s="20"/>
+      <c r="K4" s="18">
         <v>4</v>
       </c>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18">
+      <c r="L4" s="19"/>
+      <c r="M4" s="19">
         <v>7</v>
       </c>
-      <c r="N4" s="23"/>
-      <c r="O4" s="17">
-        <v>6</v>
-      </c>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18">
-        <v>5</v>
-      </c>
-      <c r="R4" s="23"/>
-      <c r="S4" s="17">
+      <c r="N4" s="20"/>
+      <c r="O4" s="18">
+        <v>6</v>
+      </c>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19">
+        <v>5</v>
+      </c>
+      <c r="R4" s="20"/>
+      <c r="S4" s="18">
         <v>9</v>
       </c>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18">
+      <c r="T4" s="19"/>
+      <c r="U4" s="19">
         <v>2</v>
       </c>
-      <c r="V4" s="23"/>
-      <c r="W4" s="17">
+      <c r="V4" s="20"/>
+      <c r="W4" s="18">
         <v>4</v>
       </c>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18">
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19">
         <v>7</v>
       </c>
-      <c r="Z4" s="18"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="18">
+        <v>6</v>
+      </c>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19">
+        <v>5</v>
+      </c>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="18">
+        <v>6</v>
+      </c>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19">
+        <v>5</v>
+      </c>
+      <c r="AH4" s="20"/>
+      <c r="AI4" s="18">
+        <v>5</v>
+      </c>
+      <c r="AJ4" s="19"/>
+      <c r="AK4" s="19">
+        <v>6</v>
+      </c>
+      <c r="AL4" s="20"/>
+      <c r="AM4" s="18">
+        <v>6</v>
+      </c>
+      <c r="AN4" s="19"/>
+      <c r="AO4" s="19">
+        <v>5</v>
+      </c>
+      <c r="AP4" s="20"/>
+      <c r="AQ4" s="5">
+        <f>AM4+AI4+AE4+AA4+W4+S4+O4+K4+G4+C4</f>
+        <v>63</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:43" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="20">
-        <v>6</v>
-      </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20">
-        <v>5</v>
-      </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="19">
+      <c r="C5" s="22">
+        <v>6</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22">
+        <v>5</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="21">
         <v>8</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20">
+      <c r="H5" s="22"/>
+      <c r="I5" s="22">
         <v>3</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="19">
+      <c r="J5" s="23"/>
+      <c r="K5" s="21">
         <v>4</v>
       </c>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20">
+      <c r="L5" s="22"/>
+      <c r="M5" s="22">
         <v>7</v>
       </c>
-      <c r="N5" s="25"/>
-      <c r="O5" s="19">
+      <c r="N5" s="23"/>
+      <c r="O5" s="21">
         <v>7</v>
       </c>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20">
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22">
         <v>4</v>
       </c>
-      <c r="R5" s="25"/>
-      <c r="S5" s="19">
+      <c r="R5" s="23"/>
+      <c r="S5" s="21">
         <v>10</v>
       </c>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20">
+      <c r="T5" s="22"/>
+      <c r="U5" s="22">
         <v>1</v>
       </c>
-      <c r="V5" s="25"/>
-      <c r="W5" s="19">
+      <c r="V5" s="23"/>
+      <c r="W5" s="21">
         <v>2</v>
       </c>
-      <c r="X5" s="20"/>
-      <c r="Y5" s="20">
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22">
         <v>9</v>
       </c>
-      <c r="Z5" s="20"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="21">
+        <v>7</v>
+      </c>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22">
+        <v>4</v>
+      </c>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="21">
+        <v>5</v>
+      </c>
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="22">
+        <v>6</v>
+      </c>
+      <c r="AH5" s="23"/>
+      <c r="AI5" s="21">
+        <v>6</v>
+      </c>
+      <c r="AJ5" s="22"/>
+      <c r="AK5" s="22">
+        <v>5</v>
+      </c>
+      <c r="AL5" s="23"/>
+      <c r="AM5" s="21">
+        <v>6</v>
+      </c>
+      <c r="AN5" s="22"/>
+      <c r="AO5" s="22">
+        <v>5</v>
+      </c>
+      <c r="AP5" s="23"/>
+      <c r="AQ5" s="5">
+        <f>AM5+AI5+AE5+AA5+W5+S5+O5+K5+G5+C5</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="26:26" x14ac:dyDescent="0.3">
+      <c r="Z22" s="26"/>
+    </row>
+    <row r="23" spans="26:26" x14ac:dyDescent="0.3">
+      <c r="Z23" s="26"/>
+    </row>
+    <row r="24" spans="26:26" x14ac:dyDescent="0.3">
+      <c r="Z24" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
+  <mergeCells count="51">
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:V5">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W4:Z5">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA4:AD5">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE4:AH5">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI4:AL5">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1067,7 +1352,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W4:Z5">
+  <conditionalFormatting sqref="AM4:AP5">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>